<commit_message>
INC0801753 - Update Package for UiAutomationActivities to 22.10.7
</commit_message>
<xml_diff>
--- a/Data/Capybara_Fin009_OutputReport_Config.xlsx
+++ b/Data/Capybara_Fin009_OutputReport_Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>Fin009-Account Receivable- System Exception</t>
+  </si>
+  <si>
+    <t>SmallDelay</t>
   </si>
 </sst>
 </file>
@@ -766,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2024,7 +2027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3280,8 +3283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3372,7 +3375,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>